<commit_message>
generated weibull constants for 1100x simulations
</commit_message>
<xml_diff>
--- a/Weibull_constants.xlsx
+++ b/Weibull_constants.xlsx
@@ -429,10 +429,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5.880905357653295</v>
+        <v>5.855461368907875</v>
       </c>
       <c r="C2">
-        <v>-2.8885487514333</v>
+        <v>0.05571496487019689</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -440,10 +440,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>5.701502819138431</v>
+        <v>5.373821717978156</v>
       </c>
       <c r="C3">
-        <v>-2.962539966166968</v>
+        <v>0.0509700646315515</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -451,10 +451,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>5.296625510618581</v>
+        <v>5.39224651444028</v>
       </c>
       <c r="C4">
-        <v>-3.04001689701093</v>
+        <v>0.04786369706241319</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -462,10 +462,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>5.142310913642156</v>
+        <v>5.242322013566242</v>
       </c>
       <c r="C5">
-        <v>-3.101414405392977</v>
+        <v>0.04518225044339162</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -473,10 +473,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>5.254137998953712</v>
+        <v>5.250397634109723</v>
       </c>
       <c r="C6">
-        <v>-3.121881000028289</v>
+        <v>0.04377345463725519</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -484,10 +484,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>5.363075626800655</v>
+        <v>5.209812860701463</v>
       </c>
       <c r="C7">
-        <v>-3.17038830914721</v>
+        <v>0.04182734253918256</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -495,10 +495,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>4.982759754783355</v>
+        <v>4.823498661210245</v>
       </c>
       <c r="C8">
-        <v>-3.194492197354258</v>
+        <v>0.04071928958785433</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -506,10 +506,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>5.090495833790516</v>
+        <v>5.06411657742001</v>
       </c>
       <c r="C9">
-        <v>-3.220323537312838</v>
+        <v>0.03963256045586165</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -517,10 +517,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>4.761974078999953</v>
+        <v>4.852897753594312</v>
       </c>
       <c r="C10">
-        <v>-3.243238071456326</v>
+        <v>0.03897010148013704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>